<commit_message>
find and fix short streams
</commit_message>
<xml_diff>
--- a/tdxhydrorapid/network_data/processing_options.xlsx
+++ b/tdxhydrorapid/network_data/processing_options.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchales/Code/tdxhydro-rapid/tdxhydrorapid/network_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchales/code/tdxhydro-rapid/tdxhydrorapid/network_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{17B8D710-4A78-D34B-8371-E3D0BF641722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219EB56C-D143-E84D-B435-500557DF779C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32840" yWindow="500" windowWidth="35960" windowHeight="27220"/>
+    <workbookView xWindow="32840" yWindow="500" windowWidth="35960" windowHeight="27220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="region_label_numbers" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>min_stream_order</t>
   </si>
@@ -51,11 +51,14 @@
   <si>
     <t>min_area_km2</t>
   </si>
+  <si>
+    <t>merge_short_streams</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -545,9 +548,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -904,12 +906,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,14 +920,14 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -938,10 +940,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
@@ -953,8 +955,11 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1020000010</v>
       </c>
@@ -967,10 +972,10 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
@@ -982,8 +987,11 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1020011530</v>
       </c>
@@ -996,10 +1004,10 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
@@ -1011,8 +1019,11 @@
       <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1020018110</v>
       </c>
@@ -1025,10 +1036,10 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
@@ -1040,8 +1051,11 @@
       <c r="I4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1020021940</v>
       </c>
@@ -1054,10 +1068,10 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
       <c r="G5">
@@ -1069,37 +1083,43 @@
       <c r="I5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>1020027430</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>15</v>
       </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
         <v>200</v>
       </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1020034170</v>
       </c>
@@ -1112,10 +1132,10 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
@@ -1127,66 +1147,75 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>1020035180</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>17</v>
       </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="3">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
         <v>50</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>1020040190</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>18</v>
       </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
         <v>3</v>
       </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
         <v>200</v>
       </c>
-      <c r="I9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2020000010</v>
       </c>
@@ -1199,10 +1228,10 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
       <c r="G10">
@@ -1214,8 +1243,11 @@
       <c r="I10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2020003440</v>
       </c>
@@ -1228,10 +1260,10 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
       <c r="G11">
@@ -1243,8 +1275,11 @@
       <c r="I11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020018240</v>
       </c>
@@ -1257,10 +1292,10 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>2</v>
       </c>
       <c r="G12">
@@ -1272,8 +1307,11 @@
       <c r="I12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2020024230</v>
       </c>
@@ -1286,10 +1324,10 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>2</v>
       </c>
       <c r="G13">
@@ -1301,8 +1339,11 @@
       <c r="I13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2020033490</v>
       </c>
@@ -1315,10 +1356,10 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>2</v>
       </c>
       <c r="G14">
@@ -1330,8 +1371,11 @@
       <c r="I14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2020065840</v>
       </c>
@@ -1344,10 +1388,10 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>2</v>
       </c>
       <c r="G15">
@@ -1359,37 +1403,43 @@
       <c r="I15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>2020071190</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>29</v>
       </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
         <v>3</v>
       </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
         <v>200</v>
       </c>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3020000010</v>
       </c>
@@ -1402,10 +1452,10 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>2</v>
       </c>
       <c r="G17">
@@ -1417,8 +1467,11 @@
       <c r="I17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3020003790</v>
       </c>
@@ -1431,10 +1484,10 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>2</v>
       </c>
       <c r="G18">
@@ -1446,8 +1499,11 @@
       <c r="I18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3020008670</v>
       </c>
@@ -1460,10 +1516,10 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>2</v>
       </c>
       <c r="G19">
@@ -1475,37 +1531,43 @@
       <c r="I19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>3020024310</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>36</v>
       </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
         <v>3</v>
       </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
         <v>200</v>
       </c>
-      <c r="I20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4020000010</v>
       </c>
@@ -1518,10 +1580,10 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>2</v>
       </c>
       <c r="G21">
@@ -1533,8 +1595,11 @@
       <c r="I21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4020006940</v>
       </c>
@@ -1547,10 +1612,10 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
         <v>2</v>
       </c>
       <c r="G22">
@@ -1562,8 +1627,11 @@
       <c r="I22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4020015090</v>
       </c>
@@ -1576,10 +1644,10 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <v>2</v>
       </c>
       <c r="G23">
@@ -1591,8 +1659,11 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4020024190</v>
       </c>
@@ -1605,10 +1676,10 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <v>2</v>
       </c>
       <c r="G24">
@@ -1620,66 +1691,75 @@
       <c r="I24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>4020034510</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>45</v>
       </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
         <v>0</v>
       </c>
-      <c r="F25" s="3">
-        <v>2</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1</v>
-      </c>
-      <c r="H25" s="3">
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
         <v>25</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>4020050210</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>46</v>
       </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
         <v>3</v>
       </c>
-      <c r="G26" s="2">
-        <v>1</v>
-      </c>
-      <c r="H26" s="2">
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
         <v>200</v>
       </c>
-      <c r="I26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4020050220</v>
       </c>
@@ -1692,10 +1772,10 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
         <v>2</v>
       </c>
       <c r="G27">
@@ -1707,182 +1787,203 @@
       <c r="I27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="J27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>4020050290</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>48</v>
       </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
         <v>3</v>
       </c>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2">
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
         <v>200</v>
       </c>
-      <c r="I28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>4020050470</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>49</v>
       </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2">
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
         <v>3</v>
       </c>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
-      <c r="H29" s="2">
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
         <v>200</v>
       </c>
-      <c r="I29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>5020000010</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>51</v>
       </c>
-      <c r="C30" s="3">
-        <v>1</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
         <v>0</v>
       </c>
-      <c r="F30" s="3">
-        <v>2</v>
-      </c>
-      <c r="G30" s="3">
-        <v>1</v>
-      </c>
-      <c r="H30" s="3">
+      <c r="F30" s="2">
+        <v>2</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
         <v>25</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="J30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
         <v>5020015660</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>52</v>
       </c>
-      <c r="C31" s="3">
-        <v>1</v>
-      </c>
-      <c r="D31" s="3">
-        <v>1</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
         <v>0</v>
       </c>
-      <c r="F31" s="3">
-        <v>2</v>
-      </c>
-      <c r="G31" s="3">
-        <v>1</v>
-      </c>
-      <c r="H31" s="3">
+      <c r="F31" s="2">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
         <v>25</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>5020037270</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>53</v>
       </c>
-      <c r="C32" s="3">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
         <v>0</v>
       </c>
-      <c r="F32" s="3">
-        <v>2</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1</v>
-      </c>
-      <c r="H32" s="3">
+      <c r="F32" s="2">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
         <v>25</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>5020049720</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>54</v>
       </c>
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2">
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
         <v>3</v>
       </c>
-      <c r="G33" s="2">
-        <v>1</v>
-      </c>
-      <c r="H33" s="2">
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
         <v>200</v>
       </c>
-      <c r="I33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>5020082270</v>
       </c>
@@ -1895,10 +1996,10 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" s="1">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <v>2</v>
       </c>
       <c r="G34">
@@ -1910,8 +2011,11 @@
       <c r="I34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6020000010</v>
       </c>
@@ -1924,10 +2028,10 @@
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <v>2</v>
       </c>
       <c r="G35">
@@ -1939,8 +2043,11 @@
       <c r="I35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6020006540</v>
       </c>
@@ -1953,10 +2060,10 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
-      <c r="F36" s="1">
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
         <v>2</v>
       </c>
       <c r="G36">
@@ -1968,8 +2075,11 @@
       <c r="I36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6020008320</v>
       </c>
@@ -1982,10 +2092,10 @@
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37" s="1">
-        <v>1</v>
-      </c>
-      <c r="F37" s="1">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>2</v>
       </c>
       <c r="G37">
@@ -1997,8 +2107,11 @@
       <c r="I37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>6020014330</v>
       </c>
@@ -2011,10 +2124,10 @@
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
         <v>2</v>
       </c>
       <c r="G38">
@@ -2026,8 +2139,11 @@
       <c r="I38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>6020017370</v>
       </c>
@@ -2040,10 +2156,10 @@
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="E39" s="1">
-        <v>1</v>
-      </c>
-      <c r="F39" s="1">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
         <v>2</v>
       </c>
       <c r="G39">
@@ -2055,8 +2171,11 @@
       <c r="I39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>6020021870</v>
       </c>
@@ -2069,10 +2188,10 @@
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="E40" s="1">
-        <v>1</v>
-      </c>
-      <c r="F40" s="1">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
         <v>2</v>
       </c>
       <c r="G40">
@@ -2084,8 +2203,11 @@
       <c r="I40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>6020029280</v>
       </c>
@@ -2098,10 +2220,10 @@
       <c r="D41">
         <v>1</v>
       </c>
-      <c r="E41" s="1">
-        <v>1</v>
-      </c>
-      <c r="F41" s="1">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
         <v>2</v>
       </c>
       <c r="G41">
@@ -2113,8 +2235,11 @@
       <c r="I41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>7020000010</v>
       </c>
@@ -2127,10 +2252,10 @@
       <c r="D42">
         <v>1</v>
       </c>
-      <c r="E42" s="1">
-        <v>1</v>
-      </c>
-      <c r="F42" s="1">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
         <v>2</v>
       </c>
       <c r="G42">
@@ -2142,8 +2267,11 @@
       <c r="I42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>7020014250</v>
       </c>
@@ -2156,10 +2284,10 @@
       <c r="D43">
         <v>1</v>
       </c>
-      <c r="E43" s="1">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1">
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
         <v>2</v>
       </c>
       <c r="G43">
@@ -2171,37 +2299,43 @@
       <c r="I43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>7020021430</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>73</v>
       </c>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2">
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
         <v>3</v>
       </c>
-      <c r="G44" s="2">
-        <v>1</v>
-      </c>
-      <c r="H44" s="2">
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
         <v>200</v>
       </c>
-      <c r="I44" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I44" s="1">
+        <v>1</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>7020024600</v>
       </c>
@@ -2214,10 +2348,10 @@
       <c r="D45">
         <v>1</v>
       </c>
-      <c r="E45" s="1">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1">
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
         <v>2</v>
       </c>
       <c r="G45">
@@ -2229,8 +2363,11 @@
       <c r="I45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>7020038340</v>
       </c>
@@ -2243,10 +2380,10 @@
       <c r="D46">
         <v>1</v>
       </c>
-      <c r="E46" s="1">
-        <v>1</v>
-      </c>
-      <c r="F46" s="1">
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
         <v>2</v>
       </c>
       <c r="G46">
@@ -2258,8 +2395,11 @@
       <c r="I46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>7020046750</v>
       </c>
@@ -2272,10 +2412,10 @@
       <c r="D47">
         <v>1</v>
       </c>
-      <c r="E47" s="1">
-        <v>1</v>
-      </c>
-      <c r="F47" s="1">
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
         <v>2</v>
       </c>
       <c r="G47">
@@ -2287,8 +2427,11 @@
       <c r="I47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>7020047840</v>
       </c>
@@ -2301,10 +2444,10 @@
       <c r="D48">
         <v>1</v>
       </c>
-      <c r="E48" s="1">
-        <v>1</v>
-      </c>
-      <c r="F48" s="1">
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
         <v>2</v>
       </c>
       <c r="G48">
@@ -2316,95 +2459,107 @@
       <c r="I48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
+      <c r="J48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
         <v>7020065090</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>78</v>
       </c>
-      <c r="C49" s="3">
-        <v>1</v>
-      </c>
-      <c r="D49" s="3">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3">
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2">
         <v>0</v>
       </c>
-      <c r="F49" s="3">
-        <v>2</v>
-      </c>
-      <c r="G49" s="3">
-        <v>1</v>
-      </c>
-      <c r="H49" s="3">
+      <c r="F49" s="2">
+        <v>2</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1</v>
+      </c>
+      <c r="H49" s="2">
         <v>25</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+      <c r="J49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>8020000010</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>81</v>
       </c>
-      <c r="C50" s="2">
-        <v>1</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2">
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
         <v>3</v>
       </c>
-      <c r="G50" s="2">
-        <v>1</v>
-      </c>
-      <c r="H50" s="2">
+      <c r="G50" s="1">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1">
         <v>200</v>
       </c>
-      <c r="I50" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+      <c r="I50" s="1">
+        <v>1</v>
+      </c>
+      <c r="J50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>8020008900</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>82</v>
       </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2">
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
         <v>3</v>
       </c>
-      <c r="G51" s="2">
-        <v>1</v>
-      </c>
-      <c r="H51" s="2">
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1">
         <v>200</v>
       </c>
-      <c r="I51" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I51" s="1">
+        <v>1</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2020041390</v>
       </c>
@@ -2417,10 +2572,10 @@
       <c r="D52">
         <v>1</v>
       </c>
-      <c r="E52" s="1">
-        <v>1</v>
-      </c>
-      <c r="F52" s="1">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
         <v>2</v>
       </c>
       <c r="G52">
@@ -2432,8 +2587,11 @@
       <c r="I52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2020057170</v>
       </c>
@@ -2446,10 +2604,10 @@
       <c r="D53">
         <v>1</v>
       </c>
-      <c r="E53" s="1">
-        <v>1</v>
-      </c>
-      <c r="F53" s="1">
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
         <v>2</v>
       </c>
       <c r="G53">
@@ -2461,8 +2619,11 @@
       <c r="I53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3020005240</v>
       </c>
@@ -2475,10 +2636,10 @@
       <c r="D54">
         <v>1</v>
       </c>
-      <c r="E54" s="1">
-        <v>1</v>
-      </c>
-      <c r="F54" s="1">
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
         <v>2</v>
       </c>
       <c r="G54">
@@ -2490,8 +2651,11 @@
       <c r="I54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3020009320</v>
       </c>
@@ -2504,10 +2668,10 @@
       <c r="D55">
         <v>1</v>
       </c>
-      <c r="E55" s="1">
-        <v>1</v>
-      </c>
-      <c r="F55" s="1">
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
         <v>2</v>
       </c>
       <c r="G55">
@@ -2519,8 +2683,11 @@
       <c r="I55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5020054880</v>
       </c>
@@ -2533,10 +2700,10 @@
       <c r="D56">
         <v>1</v>
       </c>
-      <c r="E56" s="1">
-        <v>1</v>
-      </c>
-      <c r="F56" s="1">
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
         <v>2</v>
       </c>
       <c r="G56">
@@ -2548,8 +2715,11 @@
       <c r="I56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>5020055870</v>
       </c>
@@ -2562,10 +2732,10 @@
       <c r="D57">
         <v>1</v>
       </c>
-      <c r="E57" s="1">
-        <v>1</v>
-      </c>
-      <c r="F57" s="1">
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
         <v>2</v>
       </c>
       <c r="G57">
@@ -2577,8 +2747,11 @@
       <c r="I57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>8020010700</v>
       </c>
@@ -2591,10 +2764,10 @@
       <c r="D58">
         <v>1</v>
       </c>
-      <c r="E58" s="1">
-        <v>1</v>
-      </c>
-      <c r="F58" s="1">
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
         <v>2</v>
       </c>
       <c r="G58">
@@ -2606,8 +2779,11 @@
       <c r="I58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>8020020760</v>
       </c>
@@ -2620,10 +2796,10 @@
       <c r="D59">
         <v>1</v>
       </c>
-      <c r="E59" s="1">
-        <v>1</v>
-      </c>
-      <c r="F59" s="1">
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
         <v>2</v>
       </c>
       <c r="G59">
@@ -2635,8 +2811,11 @@
       <c r="I59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>8020022890</v>
       </c>
@@ -2649,10 +2828,10 @@
       <c r="D60">
         <v>1</v>
       </c>
-      <c r="E60" s="1">
-        <v>1</v>
-      </c>
-      <c r="F60" s="1">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
         <v>2</v>
       </c>
       <c r="G60">
@@ -2664,8 +2843,11 @@
       <c r="I60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>8020032840</v>
       </c>
@@ -2678,10 +2860,10 @@
       <c r="D61">
         <v>1</v>
       </c>
-      <c r="E61" s="1">
-        <v>1</v>
-      </c>
-      <c r="F61" s="1">
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
         <v>2</v>
       </c>
       <c r="G61">
@@ -2693,8 +2875,11 @@
       <c r="I61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>8020044560</v>
       </c>
@@ -2707,10 +2892,10 @@
       <c r="D62">
         <v>1</v>
       </c>
-      <c r="E62" s="1">
-        <v>1</v>
-      </c>
-      <c r="F62" s="1">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
         <v>2</v>
       </c>
       <c r="G62">
@@ -2722,8 +2907,11 @@
       <c r="I62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>9020000010</v>
       </c>
@@ -2736,10 +2924,10 @@
       <c r="D63">
         <v>1</v>
       </c>
-      <c r="E63" s="1">
-        <v>1</v>
-      </c>
-      <c r="F63" s="1">
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
         <v>2</v>
       </c>
       <c r="G63">
@@ -2749,6 +2937,9 @@
         <v>75</v>
       </c>
       <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
processing options table formatting
</commit_message>
<xml_diff>
--- a/tdxhydrorapid/network_data/processing_options.xlsx
+++ b/tdxhydrorapid/network_data/processing_options.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchales/code/tdxhydro-rapid/tdxhydrorapid/network_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchales/code/tdxhydro-postprocessing/tdxhydrorapid/network_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61014A16-6F3E-9A41-AA05-0732A8A52193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4259F540-F3FE-B449-9C02-C252E5DDE208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="500" windowWidth="35960" windowHeight="27220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="34560" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="region_label_numbers" sheetId="1" r:id="rId1"/>
@@ -551,10 +551,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -914,7 +915,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,11 +925,13 @@
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1106,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1020027430</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1020035180</v>
       </c>
@@ -1211,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1020040190</v>
       </c>
@@ -1456,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2020057170</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3020003790</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4020000010</v>
       </c>
@@ -1806,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4020006940</v>
       </c>
@@ -1876,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4020024190</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>4020034510</v>
       </c>
@@ -1946,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>4020050210</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4020050220</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>4020050290</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>4020050470</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>6020014330</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>7020014250</v>
       </c>
@@ -2646,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>7020021430</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>7020024600</v>
       </c>
@@ -3143,5 +3146,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>